<commit_message>
small changes in details and admin values
</commit_message>
<xml_diff>
--- a/HaverDevProject/wwwroot/templates/defect-upload-template.xlsx
+++ b/HaverDevProject/wwwroot/templates/defect-upload-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diana\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{193B49E2-D631-4060-97EA-56988653A3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2355D262-9289-4543-BD13-CAC56C0D7938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5436" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{796EB6AB-8C68-47CF-91EB-20690646CA1C}"/>
+    <workbookView xWindow="4524" yWindow="1176" windowWidth="17280" windowHeight="8880" xr2:uid="{796EB6AB-8C68-47CF-91EB-20690646CA1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,19 +36,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Defect</t>
+    <t>Description</t>
   </si>
   <si>
-    <t>Description</t>
+    <r>
+      <t>Fields marked </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> are required.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Defect </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,8 +102,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -75,6 +128,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -91,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -99,6 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,24 +496,27 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.5546875" customWidth="1"/>
     <col min="2" max="2" width="32.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1"/>
       <c r="D1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new requirements implemented in item table
</commit_message>
<xml_diff>
--- a/HaverDevProject/wwwroot/templates/defect-upload-template.xlsx
+++ b/HaverDevProject/wwwroot/templates/defect-upload-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diana\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2355D262-9289-4543-BD13-CAC56C0D7938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE71BBD4-446D-48F2-AE43-AAA64F52B79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4524" yWindow="1176" windowWidth="17280" windowHeight="8880" xr2:uid="{796EB6AB-8C68-47CF-91EB-20690646CA1C}"/>
+    <workbookView xWindow="5568" yWindow="2220" windowWidth="17280" windowHeight="8880" xr2:uid="{796EB6AB-8C68-47CF-91EB-20690646CA1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Defect </t>
+      <t xml:space="preserve">Defect Type </t>
     </r>
     <r>
       <rPr>
@@ -496,7 +496,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fixing excel and create for item defect and supplier
</commit_message>
<xml_diff>
--- a/HaverDevProject/wwwroot/templates/defect-upload-template.xlsx
+++ b/HaverDevProject/wwwroot/templates/defect-upload-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diana\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE71BBD4-446D-48F2-AE43-AAA64F52B79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABB58DB-EFFC-4E64-B9BE-C72F9C5F7710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5568" yWindow="2220" windowWidth="17280" windowHeight="8880" xr2:uid="{796EB6AB-8C68-47CF-91EB-20690646CA1C}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{796EB6AB-8C68-47CF-91EB-20690646CA1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <r>
       <t>Fields marked </t>
@@ -493,31 +490,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D3389F-2737-4AAC-865C-901D336B7C41}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="32.109375" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1"/>
+      <c r="C1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>